<commit_message>
modify data for hand
</commit_message>
<xml_diff>
--- a/diagram/Ar1_diagram.xlsx
+++ b/diagram/Ar1_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Agiat_Ikazinat\Agiat_Ikazinat\diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FA3054-5184-470F-99B7-DB68BFF726A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4280EA62-3FDF-437E-8B5E-B9A8E611F55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31050" yWindow="4110" windowWidth="21600" windowHeight="11235" xr2:uid="{8CF7E09D-69CB-4638-9570-7402B5B5296D}"/>
+    <workbookView xWindow="35970" yWindow="1425" windowWidth="21600" windowHeight="11235" xr2:uid="{8CF7E09D-69CB-4638-9570-7402B5B5296D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -90,6 +90,18 @@
   </si>
   <si>
     <t>Dir2</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>*Note</t>
+  </si>
+  <si>
+    <t>Apply roughly ~7 V</t>
   </si>
 </sst>
 </file>
@@ -105,12 +117,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -125,8 +143,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ACC81B5-716B-452C-93C8-FB91F6DFDC3F}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,7 +521,7 @@
     <col min="1" max="1" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -521,48 +540,114 @@
       <c r="F1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>180</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>180</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>180</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>180</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>180</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -570,7 +655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -590,47 +675,107 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10">
+        <v>180</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>180</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12">
+        <v>180</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13">
+        <v>180</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <v>180</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>

</xml_diff>